<commit_message>
#30 Add option to not convert text to numbers: convertTextToNumber
</commit_message>
<xml_diff>
--- a/data/regression.xlsx
+++ b/data/regression.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/starver/code/makara/excel-as-json/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3FD415-B91D-934C-9C06-9F5146D658D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174C1F8D-EA51-A14F-96EC-35C0BC411373}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21460" windowHeight="17480" xr2:uid="{9E7602DE-9476-2449-91EC-468ED163C16B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21460" windowHeight="17480" activeTab="1" xr2:uid="{9E7602DE-9476-2449-91EC-468ED163C16B}"/>
   </bookViews>
   <sheets>
     <sheet name="23" sheetId="1" r:id="rId1"/>
+    <sheet name="28" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>link</t>
   </si>
@@ -46,6 +47,18 @@
   </si>
   <si>
     <t>An array list entry should contain no entries if no non-blank entries exist</t>
+  </si>
+  <si>
+    <t>furtherInformation.icon</t>
+  </si>
+  <si>
+    <t>furtherInformation.description</t>
+  </si>
+  <si>
+    <t>button.title</t>
+  </si>
+  <si>
+    <t>button.link</t>
   </si>
 </sst>
 </file>
@@ -399,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D60D8F-67CC-FC48-85EF-87DB4EAB53F6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -441,4 +454,33 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F50D822-8723-0045-8897-CBF09142114B}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>